<commit_message>
Nuevas ubicaciones de trampas
</commit_message>
<xml_diff>
--- a/UbicacionesTrampas.xlsx
+++ b/UbicacionesTrampas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudio\GitHub\allaideas-2\trampas-barcelo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32BF2AB-C25C-47D0-B1AA-9870D62EF0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B32C0-8ABF-4CBD-8FA4-E12045E6C514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{E002C49E-E3A0-49AF-B2CC-DD45AB4EFF39}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Código</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>MVL001</t>
+  </si>
+  <si>
+    <t>uapmarcelino</t>
+  </si>
+  <si>
+    <t>uapburman</t>
+  </si>
+  <si>
+    <t>UAP Marcelino</t>
+  </si>
+  <si>
+    <t>General Lavalle 1583</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>URI Burman</t>
+  </si>
+  <si>
+    <t>Ituzaingó 5725</t>
+  </si>
+  <si>
+    <t>CARAPACHAY</t>
   </si>
 </sst>
 </file>
@@ -456,7 +480,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -547,6 +571,46 @@
         <v>-58.504440928078097</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>-34.532160508112803</v>
+      </c>
+      <c r="F5">
+        <v>-58.480465826746901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>-34.527681854771501</v>
+      </c>
+      <c r="F6">
+        <v>-58.536327416546001</v>
+      </c>
+    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9" s="3"/>
     </row>

</xml_diff>